<commit_message>
add: print formulas option(-f)
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/work/xlconv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00087ADF-A8B8-5F43-8803-03598D628787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C371920E-ADC4-4C43-9830-42520C23DF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32340" yWindow="-10200" windowWidth="28800" windowHeight="17500" xr2:uid="{B1D6F636-FA6D-8140-A81A-A725912B3599}"/>
+    <workbookView xWindow="-32340" yWindow="-3100" windowWidth="28800" windowHeight="17500" xr2:uid="{B1D6F636-FA6D-8140-A81A-A725912B3599}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,6 +50,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -95,11 +98,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -120,9 +126,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -160,7 +166,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -266,7 +272,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,7 +414,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,13 +423,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D20068-F564-9640-A50D-8FF5B06D7483}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -435,6 +444,18 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2">
+        <f ca="1">NOW()</f>
+        <v>45340.587745833334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" s="2">
+        <f ca="1">A3+DAY(1)</f>
+        <v>45341.587745833334</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>